<commit_message>
add: WordDialog and remove EN-TJ, TJ-EN word from DB
</commit_message>
<xml_diff>
--- a/forPlayMarket/actualVersion/keywordList.xlsx
+++ b/forPlayMarket/actualVersion/keywordList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\androidProject\farhang\forPlayMarket\actualVersion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15733950-187E-4F77-800C-4DBF10761C80}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C673C20A-0A0A-49D6-A963-CE04787AB95F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Ключевое слово</t>
   </si>
@@ -45,12 +45,6 @@
     <t>таджикско русский словарь</t>
   </si>
   <si>
-    <t>таджикско английский словарь</t>
-  </si>
-  <si>
-    <t>таджикско английский переводчик</t>
-  </si>
-  <si>
     <t>бесплатно русско таджикский словарь</t>
   </si>
   <si>
@@ -58,9 +52,6 @@
   </si>
   <si>
     <t>переводчик с русского на таджикский</t>
-  </si>
-  <si>
-    <t>переводчик с английского на таджикский</t>
   </si>
   <si>
     <t>ёднома</t>
@@ -421,7 +412,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,16 +428,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3">
         <v>21000</v>
@@ -455,14 +446,14 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3">
         <v>11157</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -473,6 +464,9 @@
         <v>3275</v>
       </c>
       <c r="C4" s="2"/>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -492,16 +486,11 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1292</v>
-      </c>
+      <c r="B7" s="3"/>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -513,16 +502,11 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="3">
-        <v>617</v>
-      </c>
+      <c r="B9" s="3"/>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -536,7 +520,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B11" s="3">
         <v>192</v>
@@ -545,50 +529,42 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3">
         <v>98</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="3">
-        <v>89</v>
-      </c>
+      <c r="B13" s="3"/>
       <c r="C13" s="2"/>
-      <c r="D13" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B14" s="3">
         <v>88</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3">
         <v>26</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>